<commit_message>
Add a few more deconstructions for GC-VTPR
</commit_message>
<xml_diff>
--- a/dev/GC-VTPR.xlsx
+++ b/dev/GC-VTPR.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5736" uniqueCount="4055">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5745" uniqueCount="4057">
   <si>
     <r>
       <t>Q</t>
@@ -12344,6 +12344,12 @@
   </si>
   <si>
     <t>1*303</t>
+  </si>
+  <si>
+    <t>n-Dodecane</t>
+  </si>
+  <si>
+    <t>n-Decane</t>
   </si>
 </sst>
 </file>
@@ -41146,8 +41152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M996"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="M114" sqref="A114:M114"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M37" activeCellId="2" sqref="A37 C37 M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -81986,10 +81992,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A28" sqref="A28:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -82274,6 +82280,39 @@
         <v>3319</v>
       </c>
     </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4055</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3278</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>4056</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C27" t="s">
+        <v>3265</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>140</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3252</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add a few more GC-VTPR components
</commit_message>
<xml_diff>
--- a/dev/GC-VTPR.xlsx
+++ b/dev/GC-VTPR.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5745" uniqueCount="4057">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5748" uniqueCount="4059">
   <si>
     <r>
       <t>Q</t>
@@ -12350,6 +12350,12 @@
   </si>
   <si>
     <t>n-Decane</t>
+  </si>
+  <si>
+    <t>n-Hexane</t>
+  </si>
+  <si>
+    <t>n-Pentane</t>
   </si>
 </sst>
 </file>
@@ -41152,8 +41158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M996"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M37" activeCellId="2" sqref="A37 C37 M37"/>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="M73" activeCellId="2" sqref="A73 C73 M73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -81992,10 +81998,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:C28"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -82095,7 +82101,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>332</v>
+        <v>4058</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>519</v>
@@ -82311,6 +82317,17 @@
       </c>
       <c r="C28" t="s">
         <v>3252</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>4057</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>